<commit_message>
Commit NEW practice, sentence, word timeline variables
</commit_message>
<xml_diff>
--- a/stimuli_list.xlsx
+++ b/stimuli_list.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Quentin/GitHub/Experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A95E5EA-4F09-1F4F-8EE1-A5FA7F37209D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4643C1AB-EF05-8D48-80FB-CEE4D6562CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2260" windowWidth="34460" windowHeight="24180" xr2:uid="{B9B6AF27-9868-C349-B671-7733CACE506A}"/>
+    <workbookView xWindow="18220" yWindow="3540" windowWidth="25180" windowHeight="24320" activeTab="2" xr2:uid="{B9B6AF27-9868-C349-B671-7733CACE506A}"/>
   </bookViews>
   <sheets>
     <sheet name="sentence" sheetId="1" r:id="rId1"/>
     <sheet name="word" sheetId="2" r:id="rId2"/>
+    <sheet name="practice" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2706" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2787" uniqueCount="1237">
   <si>
     <t>List 1</t>
   </si>
@@ -3861,6 +3862,179 @@
   </si>
   <si>
     <t>FAS_K9M-PBKW-03-09.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemID</t>
+  </si>
+  <si>
+    <t>Sound1</t>
+  </si>
+  <si>
+    <t>Sound2</t>
+  </si>
+  <si>
+    <t>ExpAns</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>FAS_M6M-BKBR-00-01.wav</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>FAS_M6M-BKBR-00-02.wav</t>
+  </si>
+  <si>
+    <t>FAS_M6M-BKBR-00-03.wav</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>FAS_M1M-BKBR-00-02.wav</t>
+  </si>
+  <si>
+    <t>FAS_M1M-BKBR-00-03.wav</t>
+  </si>
+  <si>
+    <t>FAS_E5M-WIPI-01-01.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E1M-WIPI-01-01.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E1M-WIPI-01-02.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E5M-WIPI-01-02.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E1M-WIPI-01-03.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E5M-WIPI-01-03.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E1M-WIPI-01-04.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_M6M-WIPI-01-04.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_M6M-WIPI-01-05.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E1M-WIPI-01-05.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E1M-WIPI-01-06.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_M6M-WIPI-01-06.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_M1M-BKBR-00-01.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>school</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ball</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>smoke</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>floor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fox</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E5M-HINT-00-01.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E5M-HINT-00-02.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_M6M-HINT-00-03.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_M6M-HINT-00-01.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_M6M-HINT-00-02.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAS_E5M-HINT-00-03.wav</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>They watched the movie.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>It is time to go home.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The tomatoes grew in his garden.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The boy got into trouble.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The yellow pears taste good.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The front yard is pretty.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WIPI</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4329,7 +4503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D41B23-73B7-9F41-A3C1-82F9DABE0114}">
   <dimension ref="A2:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -9952,7 +10126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7D2983-029A-214D-B22D-2CF3D7288A05}">
   <dimension ref="A2:I202"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -15573,4 +15747,402 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A077183A-F3BD-D24B-B238-62047086C96A}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="2" width="27" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1210</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1212</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1213</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1214</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1215</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1216</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1197</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1200</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1201</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1204</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B11" t="s">
+        <v>697</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1227</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B12" t="s">
+        <v>697</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1225</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1228</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B13" t="s">
+        <v>697</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1229</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>